<commit_message>
Just gotta fix up uncertainties now
</commit_message>
<xml_diff>
--- a/Labs/Lab 3 - Measurement of the Bandgap in Germanium/Band-Gap.xlsx
+++ b/Labs/Lab 3 - Measurement of the Bandgap in Germanium/Band-Gap.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204E6F35-A6A7-41F2-B7E3-E580374EECD4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875C0F8B-F612-4D29-ACAB-8242494403F4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="1785" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="e">Sheet1!$X$2</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>V</t>
   </si>
@@ -190,7 +191,7 @@
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="##0.00E+0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,8 +236,23 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,8 +265,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -273,11 +301,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="5"/>
+      </right>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="5"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -319,6 +409,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2008,16 +2125,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>717098</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>13607</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>517072</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>110416</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>689882</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>16527</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2442,8 +2559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EY314"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2471,27 +2588,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:155" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
       <c r="T1" s="2" t="s">
         <v>8</v>
       </c>
@@ -3104,11 +3221,11 @@
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="17" t="s">
+      <c r="T4" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
+      <c r="U4" s="26"/>
+      <c r="V4" s="26"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
@@ -53401,4 +53518,102 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD55562-95D3-420F-B890-A7983C1E409E}">
+  <dimension ref="A2:A17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="48.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>